<commit_message>
pie chart and map
</commit_message>
<xml_diff>
--- a/gender-equality-index-2005-2010-2012-2015.xlsx
+++ b/gender-equality-index-2005-2010-2012-2015.xlsx
@@ -50347,7 +50347,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -50614,7 +50614,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>